<commit_message>
Reportes de monitoreo por auditoria mayo
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-270215.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Acciones_Correctivas-270215.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5292" yWindow="2280" windowWidth="9756" windowHeight="5100"/>
+    <workbookView xWindow="5295" yWindow="2280" windowWidth="9750" windowHeight="5100"/>
   </bookViews>
   <sheets>
     <sheet name="Acciones correctivas" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Acciones correctivas</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Por falta de clientes no existen horas a registrar en la entrega de servicio.</t>
+  </si>
+  <si>
+    <t>Se comenzara con la busqueda de clientes a quienes se les brinden el servicio generado.</t>
+  </si>
+  <si>
+    <t>Fidel Reyna</t>
+  </si>
+  <si>
+    <t>Abierto</t>
   </si>
 </sst>
 </file>
@@ -146,18 +158,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -170,33 +176,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -216,6 +215,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -264,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,7 +301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -510,89 +512,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.44140625" style="2"/>
-    <col min="12" max="12" width="1.33203125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="11.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="1.28515625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-    </row>
-    <row r="2" spans="1:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5">
+        <v>42062</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="7">
+        <v>42094</v>
+      </c>
+      <c r="I5" s="13">
+        <v>42094</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -602,7 +620,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -612,7 +630,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -622,7 +640,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -632,7 +650,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -642,7 +660,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -652,7 +670,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -662,7 +680,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -672,7 +690,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -682,7 +700,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -692,7 +710,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -702,7 +720,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -712,7 +730,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -722,7 +740,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -732,7 +750,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -742,7 +760,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -752,7 +770,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -762,7 +780,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -772,7 +790,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -782,7 +800,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -792,7 +810,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -802,7 +820,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:10" ht="13.9" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -812,7 +830,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -827,12 +845,12 @@
     <mergeCell ref="A1:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:I4">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>